<commit_message>
Mon, Nov  5, 2018 11:58:52 PM
</commit_message>
<xml_diff>
--- a/Data/Summary GDA.xlsx
+++ b/Data/Summary GDA.xlsx
@@ -1,25 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\groberts\Documents\MCH Ischemia\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robertsgr\Documents\MCH_Ischemia\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C751889-83CA-4563-B44B-D36C6720E459}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7590" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
     <sheet name="Flow Rates" sheetId="2" r:id="rId2"/>
     <sheet name="Combined" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -289,7 +295,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -844,7 +850,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -952,6 +958,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -970,24 +982,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1268,11 +1275,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB101"/>
   <sheetViews>
-    <sheetView topLeftCell="K25" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="P71" workbookViewId="0">
+      <selection activeCell="X96" sqref="X96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3396,22 +3403,22 @@
         <v>54</v>
       </c>
       <c r="S48" s="11">
-        <f>(S41-S20)/AVERAGE(S21,S42)</f>
-        <v>0.28317309104172089</v>
+        <f>(S41-S20)/SQRT((S42^2+S21^2)/2)</f>
+        <v>0.27997081334390261</v>
       </c>
       <c r="U48" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="V48" s="31">
-        <f>(V30-V9)/AVERAGE(V10,V31)</f>
-        <v>0.13310931200689807</v>
+      <c r="V48" s="11">
+        <f>(V30-V9)/SQRT((V10^2+V31^2)/2)</f>
+        <v>0.13214457906276661</v>
       </c>
       <c r="X48" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="Y48" s="92">
-        <f>(Y36-Y15)/AVERAGE(Y16,Y37)</f>
-        <v>0.56739977742662218</v>
+      <c r="Y48" s="109">
+        <f>(Y36-Y15)/SQRT((Y16^2+Y37^2)/2)</f>
+        <v>0.56242970771187328</v>
       </c>
       <c r="AA48" s="30" t="s">
         <v>54</v>
@@ -4396,21 +4403,21 @@
       <c r="X73" s="42"/>
     </row>
     <row r="74" spans="1:28" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B74" s="97" t="s">
+      <c r="B74" s="99" t="s">
         <v>66</v>
       </c>
-      <c r="C74" s="98"/>
-      <c r="D74" s="99"/>
+      <c r="C74" s="100"/>
+      <c r="D74" s="101"/>
       <c r="E74" s="70" t="s">
         <v>1</v>
       </c>
       <c r="F74" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="G74" s="97" t="s">
+      <c r="G74" s="99" t="s">
         <v>67</v>
       </c>
-      <c r="H74" s="99"/>
+      <c r="H74" s="101"/>
       <c r="I74" s="85" t="s">
         <v>1</v>
       </c>
@@ -4418,21 +4425,21 @@
         <v>63</v>
       </c>
       <c r="K74" s="36"/>
-      <c r="R74" s="97" t="s">
+      <c r="R74" s="99" t="s">
         <v>66</v>
       </c>
-      <c r="S74" s="98"/>
-      <c r="T74" s="99"/>
+      <c r="S74" s="100"/>
+      <c r="T74" s="101"/>
       <c r="U74" s="70" t="s">
         <v>1</v>
       </c>
       <c r="V74" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="W74" s="97" t="s">
+      <c r="W74" s="99" t="s">
         <v>67</v>
       </c>
-      <c r="X74" s="99"/>
+      <c r="X74" s="101"/>
       <c r="Y74" s="85" t="s">
         <v>1</v>
       </c>
@@ -4441,9 +4448,9 @@
       </c>
     </row>
     <row r="75" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B75" s="100"/>
-      <c r="C75" s="101"/>
-      <c r="D75" s="102"/>
+      <c r="B75" s="102"/>
+      <c r="C75" s="103"/>
+      <c r="D75" s="104"/>
       <c r="E75" s="45" t="s">
         <v>53</v>
       </c>
@@ -4451,8 +4458,8 @@
         <f>_xlfn.T.TEST(F5:F8,B5:B19,2,3)</f>
         <v>0.83429364087293068</v>
       </c>
-      <c r="G75" s="100"/>
-      <c r="H75" s="102"/>
+      <c r="G75" s="102"/>
+      <c r="H75" s="104"/>
       <c r="I75" s="46" t="s">
         <v>53</v>
       </c>
@@ -4460,9 +4467,9 @@
         <f>_xlfn.T.TEST(J5:J14,B5:B19,2,3)</f>
         <v>0.19484929747430196</v>
       </c>
-      <c r="R75" s="100"/>
-      <c r="S75" s="101"/>
-      <c r="T75" s="102"/>
+      <c r="R75" s="102"/>
+      <c r="S75" s="103"/>
+      <c r="T75" s="104"/>
       <c r="U75" s="45" t="s">
         <v>53</v>
       </c>
@@ -4470,8 +4477,8 @@
         <f>_xlfn.T.TEST(V5:V8,S5:S19,2,3)</f>
         <v>0.79612738013523043</v>
       </c>
-      <c r="W75" s="100"/>
-      <c r="X75" s="102"/>
+      <c r="W75" s="102"/>
+      <c r="X75" s="104"/>
       <c r="Y75" s="46" t="s">
         <v>53</v>
       </c>
@@ -4481,32 +4488,38 @@
       </c>
     </row>
     <row r="76" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B76" s="100"/>
-      <c r="C76" s="101"/>
-      <c r="D76" s="102"/>
+      <c r="B76" s="102"/>
+      <c r="C76" s="103"/>
+      <c r="D76" s="104"/>
       <c r="E76" s="47" t="s">
         <v>54</v>
       </c>
       <c r="F76" s="73"/>
-      <c r="G76" s="100"/>
-      <c r="H76" s="102"/>
+      <c r="G76" s="102"/>
+      <c r="H76" s="104"/>
       <c r="I76" s="52" t="s">
         <v>54</v>
       </c>
       <c r="J76" s="86"/>
-      <c r="R76" s="100"/>
-      <c r="S76" s="101"/>
-      <c r="T76" s="102"/>
+      <c r="R76" s="102"/>
+      <c r="S76" s="103"/>
+      <c r="T76" s="104"/>
       <c r="U76" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="V76" s="73"/>
-      <c r="W76" s="100"/>
-      <c r="X76" s="102"/>
+      <c r="V76" s="73">
+        <f>(V9-S20)/SQRT((S21^2+V10^2)/2)</f>
+        <v>0.19918775571333236</v>
+      </c>
+      <c r="W76" s="102"/>
+      <c r="X76" s="104"/>
       <c r="Y76" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="Z76" s="86"/>
+      <c r="Z76" s="76">
+        <f>ABS((Y15-S20)/SQRT((Y16^2+S21^2)/2))</f>
+        <v>0.67450593704284212</v>
+      </c>
     </row>
     <row r="77" spans="1:28" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B77" s="17"/>
@@ -4628,13 +4641,19 @@
       <c r="U80" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="V80" s="76"/>
+      <c r="V80" s="76">
+        <f>(V30-S41)/SQRT((S42^2+V31^2)/2)</f>
+        <v>0.42519615443774678</v>
+      </c>
       <c r="W80" s="88"/>
       <c r="X80" s="50"/>
       <c r="Y80" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="Z80" s="73"/>
+      <c r="Z80" s="76">
+        <f>ABS((S41-Y36)/SQRT((S42^2+Y37^2)/2))</f>
+        <v>9.306809650121825E-2</v>
+      </c>
     </row>
     <row r="81" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B81" s="17"/>
@@ -4756,13 +4775,19 @@
       <c r="U84" s="79" t="s">
         <v>54</v>
       </c>
-      <c r="V84" s="80"/>
+      <c r="V84" s="80">
+        <f>ABS((V57-S68)/SQRT((S69^2+V58^2)/2))</f>
+        <v>1.3894461220121905</v>
+      </c>
       <c r="W84" s="89"/>
       <c r="X84" s="78"/>
       <c r="Y84" s="79" t="s">
         <v>54</v>
       </c>
-      <c r="Z84" s="83"/>
+      <c r="Z84" s="76">
+        <f>ABS((Y63-S68)/SQRT((Y64^2+S69^2)/2))</f>
+        <v>0.10082381644472452</v>
+      </c>
     </row>
     <row r="85" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E85" s="50"/>
@@ -4773,11 +4798,11 @@
       <c r="W85" s="16"/>
     </row>
     <row r="86" spans="2:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B86" s="97" t="s">
+      <c r="B86" s="99" t="s">
         <v>65</v>
       </c>
-      <c r="C86" s="98"/>
-      <c r="D86" s="99"/>
+      <c r="C86" s="100"/>
+      <c r="D86" s="101"/>
       <c r="E86" s="70" t="s">
         <v>1</v>
       </c>
@@ -4785,11 +4810,11 @@
         <v>63</v>
       </c>
       <c r="G86" s="36"/>
-      <c r="R86" s="97" t="s">
+      <c r="R86" s="99" t="s">
         <v>65</v>
       </c>
-      <c r="S86" s="98"/>
-      <c r="T86" s="99"/>
+      <c r="S86" s="100"/>
+      <c r="T86" s="101"/>
       <c r="U86" s="70" t="s">
         <v>1</v>
       </c>
@@ -4799,9 +4824,9 @@
       <c r="W86" s="36"/>
     </row>
     <row r="87" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B87" s="100"/>
-      <c r="C87" s="101"/>
-      <c r="D87" s="102"/>
+      <c r="B87" s="102"/>
+      <c r="C87" s="103"/>
+      <c r="D87" s="104"/>
       <c r="E87" s="45" t="s">
         <v>53</v>
       </c>
@@ -4810,9 +4835,9 @@
         <v>0.66222788810523392</v>
       </c>
       <c r="G87" s="16"/>
-      <c r="R87" s="100"/>
-      <c r="S87" s="101"/>
-      <c r="T87" s="102"/>
+      <c r="R87" s="102"/>
+      <c r="S87" s="103"/>
+      <c r="T87" s="104"/>
       <c r="U87" s="45" t="s">
         <v>53</v>
       </c>
@@ -4823,21 +4848,24 @@
       <c r="W87" s="16"/>
     </row>
     <row r="88" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B88" s="100"/>
-      <c r="C88" s="101"/>
-      <c r="D88" s="102"/>
+      <c r="B88" s="102"/>
+      <c r="C88" s="103"/>
+      <c r="D88" s="104"/>
       <c r="E88" s="53" t="s">
         <v>54</v>
       </c>
       <c r="F88" s="73"/>
       <c r="G88" s="16"/>
-      <c r="R88" s="100"/>
-      <c r="S88" s="101"/>
-      <c r="T88" s="102"/>
+      <c r="R88" s="102"/>
+      <c r="S88" s="103"/>
+      <c r="T88" s="104"/>
       <c r="U88" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="V88" s="73"/>
+      <c r="V88" s="76">
+        <f>ABS((V9-Y15)/SQRT((V10^2+Y16^2)/2))</f>
+        <v>0.38675354269306689</v>
+      </c>
       <c r="W88" s="16"/>
     </row>
     <row r="89" spans="2:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4915,7 +4943,10 @@
       <c r="U92" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="V92" s="73"/>
+      <c r="V92" s="76">
+        <f>ABS((V30-Y36)/SQRT((V31^2+Y37^2)/2))</f>
+        <v>0.34226865827209324</v>
+      </c>
       <c r="W92" s="16"/>
     </row>
     <row r="93" spans="2:26" x14ac:dyDescent="0.25">
@@ -4993,7 +5024,10 @@
       <c r="U96" s="82" t="s">
         <v>54</v>
       </c>
-      <c r="V96" s="83"/>
+      <c r="V96" s="76">
+        <f>ABS((V57-Y63)/SQRT((V58^2+Y64^2)/2))</f>
+        <v>0.50456471299066574</v>
+      </c>
       <c r="W96" s="16"/>
     </row>
     <row r="101" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5066,7 +5100,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y63 V57">
+  <conditionalFormatting sqref="V57 Y63">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="-100"/>
@@ -5107,11 +5141,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6446,21 +6480,21 @@
       <c r="G73" s="42"/>
     </row>
     <row r="74" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="97" t="s">
+      <c r="A74" s="99" t="s">
         <v>66</v>
       </c>
-      <c r="B74" s="98"/>
-      <c r="C74" s="99"/>
+      <c r="B74" s="100"/>
+      <c r="C74" s="101"/>
       <c r="D74" s="70" t="s">
         <v>1</v>
       </c>
       <c r="E74" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="F74" s="97" t="s">
+      <c r="F74" s="99" t="s">
         <v>67</v>
       </c>
-      <c r="G74" s="99"/>
+      <c r="G74" s="101"/>
       <c r="H74" s="85" t="s">
         <v>1</v>
       </c>
@@ -6469,17 +6503,17 @@
       </c>
     </row>
     <row r="75" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="100"/>
-      <c r="B75" s="101"/>
-      <c r="C75" s="102"/>
+      <c r="A75" s="102"/>
+      <c r="B75" s="103"/>
+      <c r="C75" s="104"/>
       <c r="D75" s="45" t="s">
         <v>53</v>
       </c>
       <c r="E75" s="72">
         <v>0.79612738013523043</v>
       </c>
-      <c r="F75" s="100"/>
-      <c r="G75" s="102"/>
+      <c r="F75" s="102"/>
+      <c r="G75" s="104"/>
       <c r="H75" s="46" t="s">
         <v>53</v>
       </c>
@@ -6488,15 +6522,15 @@
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" s="100"/>
-      <c r="B76" s="101"/>
-      <c r="C76" s="102"/>
+      <c r="A76" s="102"/>
+      <c r="B76" s="103"/>
+      <c r="C76" s="104"/>
       <c r="D76" s="47" t="s">
         <v>54</v>
       </c>
       <c r="E76" s="73"/>
-      <c r="F76" s="100"/>
-      <c r="G76" s="102"/>
+      <c r="F76" s="102"/>
+      <c r="G76" s="104"/>
       <c r="H76" s="52" t="s">
         <v>54</v>
       </c>
@@ -6636,11 +6670,11 @@
       <c r="F85" s="16"/>
     </row>
     <row r="86" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="97" t="s">
+      <c r="A86" s="99" t="s">
         <v>65</v>
       </c>
-      <c r="B86" s="98"/>
-      <c r="C86" s="99"/>
+      <c r="B86" s="100"/>
+      <c r="C86" s="101"/>
       <c r="D86" s="70" t="s">
         <v>1</v>
       </c>
@@ -6650,9 +6684,9 @@
       <c r="F86" s="36"/>
     </row>
     <row r="87" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="100"/>
-      <c r="B87" s="101"/>
-      <c r="C87" s="102"/>
+      <c r="A87" s="102"/>
+      <c r="B87" s="103"/>
+      <c r="C87" s="104"/>
       <c r="D87" s="45" t="s">
         <v>53</v>
       </c>
@@ -6662,9 +6696,9 @@
       <c r="F87" s="16"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" s="100"/>
-      <c r="B88" s="101"/>
-      <c r="C88" s="102"/>
+      <c r="A88" s="102"/>
+      <c r="B88" s="103"/>
+      <c r="C88" s="104"/>
       <c r="D88" s="53" t="s">
         <v>54</v>
       </c>
@@ -6785,7 +6819,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H63 E57">
+  <conditionalFormatting sqref="E57 H63">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="-100"/>
@@ -6827,7 +6861,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O96"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
@@ -6880,13 +6914,13 @@
         <v>63</v>
       </c>
       <c r="F4" s="7"/>
-      <c r="K4" s="108" t="s">
+      <c r="K4" s="105" t="s">
         <v>82</v>
       </c>
-      <c r="L4" s="108"/>
-      <c r="M4" s="108"/>
-      <c r="N4" s="108"/>
-      <c r="O4" s="108"/>
+      <c r="L4" s="105"/>
+      <c r="M4" s="105"/>
+      <c r="N4" s="105"/>
+      <c r="O4" s="105"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
@@ -6901,22 +6935,22 @@
       <c r="E5" s="13">
         <v>-204.41326846953166</v>
       </c>
-      <c r="F5" s="105" t="s">
+      <c r="F5" s="106" t="s">
         <v>73</v>
       </c>
-      <c r="G5" s="104"/>
-      <c r="H5" s="104"/>
+      <c r="G5" s="107"/>
+      <c r="H5" s="107"/>
       <c r="K5" s="95" t="s">
         <v>7</v>
       </c>
       <c r="L5" s="13">
         <v>-204.41326846953166</v>
       </c>
-      <c r="M5" s="105" t="s">
+      <c r="M5" s="106" t="s">
         <v>73</v>
       </c>
-      <c r="N5" s="104"/>
-      <c r="O5" s="104"/>
+      <c r="N5" s="107"/>
+      <c r="O5" s="107"/>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
@@ -6931,22 +6965,22 @@
       <c r="E6" s="13">
         <v>120.85244052933399</v>
       </c>
-      <c r="F6" s="105" t="s">
+      <c r="F6" s="106" t="s">
         <v>73</v>
       </c>
-      <c r="G6" s="104"/>
-      <c r="H6" s="104"/>
+      <c r="G6" s="107"/>
+      <c r="H6" s="107"/>
       <c r="K6" s="13" t="s">
         <v>12</v>
       </c>
       <c r="L6" s="13">
         <v>120.85244052933399</v>
       </c>
-      <c r="M6" s="105" t="s">
+      <c r="M6" s="106" t="s">
         <v>73</v>
       </c>
-      <c r="N6" s="104"/>
-      <c r="O6" s="104"/>
+      <c r="N6" s="107"/>
+      <c r="O6" s="107"/>
     </row>
     <row r="7" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
@@ -6961,22 +6995,22 @@
       <c r="E7" s="13">
         <v>-240.17138163193698</v>
       </c>
-      <c r="F7" s="105" t="s">
+      <c r="F7" s="106" t="s">
         <v>74</v>
       </c>
-      <c r="G7" s="104"/>
-      <c r="H7" s="104"/>
+      <c r="G7" s="107"/>
+      <c r="H7" s="107"/>
       <c r="K7" s="95" t="s">
         <v>43</v>
       </c>
       <c r="L7" s="13">
         <v>92.53518966457726</v>
       </c>
-      <c r="M7" s="105" t="s">
+      <c r="M7" s="106" t="s">
         <v>73</v>
       </c>
-      <c r="N7" s="104"/>
-      <c r="O7" s="104"/>
+      <c r="N7" s="107"/>
+      <c r="O7" s="107"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
@@ -6991,22 +7025,22 @@
       <c r="E8" s="13">
         <v>937.89820907570538</v>
       </c>
-      <c r="F8" s="105" t="s">
+      <c r="F8" s="106" t="s">
         <v>80</v>
       </c>
-      <c r="G8" s="104"/>
-      <c r="H8" s="104"/>
+      <c r="G8" s="107"/>
+      <c r="H8" s="107"/>
       <c r="K8" s="13" t="s">
         <v>45</v>
       </c>
       <c r="L8" s="13">
         <v>91.563377374129416</v>
       </c>
-      <c r="M8" s="105" t="s">
+      <c r="M8" s="106" t="s">
         <v>73</v>
       </c>
-      <c r="N8" s="104"/>
-      <c r="O8" s="104"/>
+      <c r="N8" s="107"/>
+      <c r="O8" s="107"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -7021,16 +7055,16 @@
       <c r="E9" s="13">
         <v>110.27258157435739</v>
       </c>
-      <c r="F9" s="105" t="s">
+      <c r="F9" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="G9" s="104"/>
-      <c r="H9" s="104"/>
+      <c r="G9" s="107"/>
+      <c r="H9" s="107"/>
       <c r="K9" s="50"/>
       <c r="L9" s="50"/>
-      <c r="M9" s="106"/>
-      <c r="N9" s="103"/>
-      <c r="O9" s="103"/>
+      <c r="M9" s="98"/>
+      <c r="N9" s="97"/>
+      <c r="O9" s="97"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -7047,9 +7081,9 @@
       </c>
       <c r="K10" s="50"/>
       <c r="L10" s="50"/>
-      <c r="M10" s="106"/>
-      <c r="N10" s="103"/>
-      <c r="O10" s="103"/>
+      <c r="M10" s="98"/>
+      <c r="N10" s="97"/>
+      <c r="O10" s="97"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
@@ -7064,13 +7098,13 @@
       <c r="E11" s="13">
         <v>89.698925848177623</v>
       </c>
-      <c r="K11" s="108" t="s">
+      <c r="K11" s="105" t="s">
         <v>83</v>
       </c>
-      <c r="L11" s="108"/>
-      <c r="M11" s="108"/>
-      <c r="N11" s="108"/>
-      <c r="O11" s="108"/>
+      <c r="L11" s="105"/>
+      <c r="M11" s="105"/>
+      <c r="N11" s="105"/>
+      <c r="O11" s="105"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
@@ -7085,22 +7119,22 @@
       <c r="E12" s="13">
         <v>86.300113483264099</v>
       </c>
-      <c r="F12" s="105" t="s">
+      <c r="F12" s="106" t="s">
         <v>77</v>
       </c>
-      <c r="G12" s="104"/>
-      <c r="H12" s="104"/>
+      <c r="G12" s="107"/>
+      <c r="H12" s="107"/>
       <c r="K12" s="94" t="s">
         <v>36</v>
       </c>
       <c r="L12" s="13">
         <v>-131.89988980258138</v>
       </c>
-      <c r="M12" s="105" t="s">
+      <c r="M12" s="106" t="s">
         <v>78</v>
       </c>
-      <c r="N12" s="104"/>
-      <c r="O12" s="104"/>
+      <c r="N12" s="107"/>
+      <c r="O12" s="107"/>
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
@@ -7115,22 +7149,22 @@
       <c r="E13" s="13">
         <v>-166.94515408677509</v>
       </c>
-      <c r="F13" s="105" t="s">
+      <c r="F13" s="106" t="s">
         <v>78</v>
       </c>
-      <c r="G13" s="104"/>
-      <c r="H13" s="104"/>
+      <c r="G13" s="107"/>
+      <c r="H13" s="107"/>
       <c r="K13" s="94" t="s">
         <v>36</v>
       </c>
       <c r="L13" s="13">
         <v>-35.209092636503023</v>
       </c>
-      <c r="M13" s="105" t="s">
+      <c r="M13" s="106" t="s">
         <v>78</v>
       </c>
-      <c r="N13" s="104"/>
-      <c r="O13" s="104"/>
+      <c r="N13" s="107"/>
+      <c r="O13" s="107"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
@@ -7145,22 +7179,22 @@
       <c r="E14" s="13">
         <v>-92.575768832528084</v>
       </c>
-      <c r="F14" s="105" t="s">
+      <c r="F14" s="106" t="s">
         <v>79</v>
       </c>
-      <c r="G14" s="104"/>
-      <c r="H14" s="104"/>
+      <c r="G14" s="107"/>
+      <c r="H14" s="107"/>
       <c r="K14" s="93" t="s">
         <v>34</v>
       </c>
       <c r="L14" s="13">
         <v>-236.73173748573311</v>
       </c>
-      <c r="M14" s="105" t="s">
+      <c r="M14" s="106" t="s">
         <v>78</v>
       </c>
-      <c r="N14" s="107"/>
-      <c r="O14" s="107"/>
+      <c r="N14" s="108"/>
+      <c r="O14" s="108"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
@@ -7175,22 +7209,22 @@
       <c r="E15" s="13">
         <v>-83.419333217354989</v>
       </c>
-      <c r="F15" s="105" t="s">
+      <c r="F15" s="106" t="s">
         <v>79</v>
       </c>
-      <c r="G15" s="104"/>
-      <c r="H15" s="104"/>
+      <c r="G15" s="107"/>
+      <c r="H15" s="107"/>
       <c r="K15" s="93" t="s">
         <v>55</v>
       </c>
       <c r="L15" s="13">
         <v>-138.34234368952491</v>
       </c>
-      <c r="M15" s="105" t="s">
+      <c r="M15" s="106" t="s">
         <v>78</v>
       </c>
-      <c r="N15" s="107"/>
-      <c r="O15" s="107"/>
+      <c r="N15" s="108"/>
+      <c r="O15" s="108"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
@@ -7205,22 +7239,22 @@
       <c r="E16" s="13">
         <v>133.54048634274659</v>
       </c>
-      <c r="F16" s="105" t="s">
+      <c r="F16" s="106" t="s">
         <v>81</v>
       </c>
-      <c r="G16" s="104"/>
-      <c r="H16" s="104"/>
+      <c r="G16" s="107"/>
+      <c r="H16" s="107"/>
       <c r="K16" s="93" t="s">
         <v>27</v>
       </c>
       <c r="L16" s="13">
         <v>-166.94515408677509</v>
       </c>
-      <c r="M16" s="105" t="s">
+      <c r="M16" s="106" t="s">
         <v>78</v>
       </c>
-      <c r="N16" s="104"/>
-      <c r="O16" s="104"/>
+      <c r="N16" s="107"/>
+      <c r="O16" s="107"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
@@ -7235,22 +7269,22 @@
       <c r="E17" s="13">
         <v>-236.73173748573311</v>
       </c>
-      <c r="F17" s="105" t="s">
+      <c r="F17" s="106" t="s">
         <v>78</v>
       </c>
-      <c r="G17" s="107"/>
-      <c r="H17" s="107"/>
+      <c r="G17" s="108"/>
+      <c r="H17" s="108"/>
       <c r="K17" s="93" t="s">
         <v>27</v>
       </c>
       <c r="L17" s="13">
         <v>-183.3714839935835</v>
       </c>
-      <c r="M17" s="105" t="s">
+      <c r="M17" s="106" t="s">
         <v>78</v>
       </c>
-      <c r="N17" s="104"/>
-      <c r="O17" s="104"/>
+      <c r="N17" s="107"/>
+      <c r="O17" s="107"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
@@ -7265,22 +7299,22 @@
       <c r="E18" s="13">
         <v>-131.89988980258138</v>
       </c>
-      <c r="F18" s="105" t="s">
+      <c r="F18" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="G18" s="104"/>
-      <c r="H18" s="104"/>
+      <c r="G18" s="107"/>
+      <c r="H18" s="107"/>
       <c r="K18" s="13" t="s">
         <v>9</v>
       </c>
       <c r="L18" s="13">
         <v>110.27258157435739</v>
       </c>
-      <c r="M18" s="105" t="s">
+      <c r="M18" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="N18" s="104"/>
-      <c r="O18" s="104"/>
+      <c r="N18" s="107"/>
+      <c r="O18" s="107"/>
     </row>
     <row r="19" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
@@ -7301,11 +7335,11 @@
       <c r="L19" s="13">
         <v>361.1808928803157</v>
       </c>
-      <c r="M19" s="105" t="s">
+      <c r="M19" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="N19" s="104"/>
-      <c r="O19" s="104"/>
+      <c r="N19" s="107"/>
+      <c r="O19" s="107"/>
     </row>
     <row r="20" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
@@ -7324,9 +7358,9 @@
       <c r="F20" s="22"/>
       <c r="K20" s="50"/>
       <c r="L20" s="50"/>
-      <c r="M20" s="106"/>
-      <c r="N20" s="103"/>
-      <c r="O20" s="103"/>
+      <c r="M20" s="98"/>
+      <c r="N20" s="97"/>
+      <c r="O20" s="97"/>
     </row>
     <row r="21" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
@@ -7351,13 +7385,13 @@
         <v>14</v>
       </c>
       <c r="F22" s="7"/>
-      <c r="K22" s="108" t="s">
+      <c r="K22" s="105" t="s">
         <v>84</v>
       </c>
-      <c r="L22" s="108"/>
-      <c r="M22" s="108"/>
-      <c r="N22" s="108"/>
-      <c r="O22" s="108"/>
+      <c r="L22" s="105"/>
+      <c r="M22" s="105"/>
+      <c r="N22" s="105"/>
+      <c r="O22" s="105"/>
     </row>
     <row r="23" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="21"/>
@@ -7369,11 +7403,11 @@
       <c r="L23" s="13">
         <v>86.300113483264099</v>
       </c>
-      <c r="M23" s="105" t="s">
+      <c r="M23" s="106" t="s">
         <v>77</v>
       </c>
-      <c r="N23" s="104"/>
-      <c r="O23" s="104"/>
+      <c r="N23" s="107"/>
+      <c r="O23" s="107"/>
     </row>
     <row r="24" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
@@ -7390,11 +7424,11 @@
       <c r="L24" s="13">
         <v>110.95469137218241</v>
       </c>
-      <c r="M24" s="105" t="s">
+      <c r="M24" s="106" t="s">
         <v>77</v>
       </c>
-      <c r="N24" s="104"/>
-      <c r="O24" s="104"/>
+      <c r="N24" s="107"/>
+      <c r="O24" s="107"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
@@ -7416,11 +7450,11 @@
       <c r="L25" s="13">
         <v>133.54048634274659</v>
       </c>
-      <c r="M25" s="105" t="s">
+      <c r="M25" s="106" t="s">
         <v>81</v>
       </c>
-      <c r="N25" s="104"/>
-      <c r="O25" s="104"/>
+      <c r="N25" s="107"/>
+      <c r="O25" s="107"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
@@ -7435,22 +7469,22 @@
       <c r="E26" s="13">
         <v>92.53518966457726</v>
       </c>
-      <c r="F26" s="105" t="s">
+      <c r="F26" s="106" t="s">
         <v>73</v>
       </c>
-      <c r="G26" s="104"/>
-      <c r="H26" s="104"/>
+      <c r="G26" s="107"/>
+      <c r="H26" s="107"/>
       <c r="K26" s="93" t="s">
         <v>33</v>
       </c>
       <c r="L26" s="13">
         <v>505.69965904746408</v>
       </c>
-      <c r="M26" s="105" t="s">
+      <c r="M26" s="106" t="s">
         <v>80</v>
       </c>
-      <c r="N26" s="104"/>
-      <c r="O26" s="104"/>
+      <c r="N26" s="107"/>
+      <c r="O26" s="107"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
@@ -7465,11 +7499,11 @@
       <c r="E27" s="13">
         <v>91.563377374129416</v>
       </c>
-      <c r="F27" s="105" t="s">
+      <c r="F27" s="106" t="s">
         <v>73</v>
       </c>
-      <c r="G27" s="104"/>
-      <c r="H27" s="104"/>
+      <c r="G27" s="107"/>
+      <c r="H27" s="107"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
@@ -7484,11 +7518,11 @@
       <c r="E28" s="13">
         <v>-149.34216837262221</v>
       </c>
-      <c r="F28" s="105" t="s">
+      <c r="F28" s="106" t="s">
         <v>74</v>
       </c>
-      <c r="G28" s="104"/>
-      <c r="H28" s="104"/>
+      <c r="G28" s="107"/>
+      <c r="H28" s="107"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
@@ -7503,18 +7537,18 @@
       <c r="E29" s="13">
         <v>839.46341018580051</v>
       </c>
-      <c r="F29" s="105" t="s">
+      <c r="F29" s="106" t="s">
         <v>75</v>
       </c>
-      <c r="G29" s="104"/>
-      <c r="H29" s="104"/>
-      <c r="K29" s="108" t="s">
+      <c r="G29" s="107"/>
+      <c r="H29" s="107"/>
+      <c r="K29" s="105" t="s">
         <v>85</v>
       </c>
-      <c r="L29" s="108"/>
-      <c r="M29" s="108"/>
-      <c r="N29" s="108"/>
-      <c r="O29" s="108"/>
+      <c r="L29" s="105"/>
+      <c r="M29" s="105"/>
+      <c r="N29" s="105"/>
+      <c r="O29" s="105"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
@@ -7530,22 +7564,22 @@
       <c r="E30" s="13">
         <v>361.1808928803157</v>
       </c>
-      <c r="F30" s="105" t="s">
+      <c r="F30" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="G30" s="104"/>
-      <c r="H30" s="104"/>
+      <c r="G30" s="107"/>
+      <c r="H30" s="107"/>
       <c r="K30" s="13" t="s">
         <v>29</v>
       </c>
       <c r="L30" s="13">
         <v>-92.575768832528084</v>
       </c>
-      <c r="M30" s="105" t="s">
+      <c r="M30" s="106" t="s">
         <v>79</v>
       </c>
-      <c r="N30" s="104"/>
-      <c r="O30" s="104"/>
+      <c r="N30" s="107"/>
+      <c r="O30" s="107"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
@@ -7567,11 +7601,11 @@
       <c r="L31" s="13">
         <v>75.812386599726835</v>
       </c>
-      <c r="M31" s="105" t="s">
+      <c r="M31" s="106" t="s">
         <v>79</v>
       </c>
-      <c r="N31" s="104"/>
-      <c r="O31" s="104"/>
+      <c r="N31" s="107"/>
+      <c r="O31" s="107"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
@@ -7593,11 +7627,11 @@
       <c r="L32" s="13">
         <v>-83.419333217354989</v>
       </c>
-      <c r="M32" s="105" t="s">
+      <c r="M32" s="106" t="s">
         <v>79</v>
       </c>
-      <c r="N32" s="104"/>
-      <c r="O32" s="104"/>
+      <c r="N32" s="107"/>
+      <c r="O32" s="107"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
@@ -7613,22 +7647,22 @@
       <c r="E33" s="13">
         <v>110.95469137218241</v>
       </c>
-      <c r="F33" s="105" t="s">
+      <c r="F33" s="106" t="s">
         <v>77</v>
       </c>
-      <c r="G33" s="104"/>
-      <c r="H33" s="104"/>
+      <c r="G33" s="107"/>
+      <c r="H33" s="107"/>
       <c r="K33" s="13" t="s">
         <v>31</v>
       </c>
       <c r="L33" s="13">
         <v>62.348001730346624</v>
       </c>
-      <c r="M33" s="105" t="s">
+      <c r="M33" s="106" t="s">
         <v>79</v>
       </c>
-      <c r="N33" s="104"/>
-      <c r="O33" s="104"/>
+      <c r="N33" s="107"/>
+      <c r="O33" s="107"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
@@ -7644,11 +7678,11 @@
       <c r="E34" s="13">
         <v>-183.3714839935835</v>
       </c>
-      <c r="F34" s="105" t="s">
+      <c r="F34" s="106" t="s">
         <v>78</v>
       </c>
-      <c r="G34" s="104"/>
-      <c r="H34" s="104"/>
+      <c r="G34" s="107"/>
+      <c r="H34" s="107"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
@@ -7663,11 +7697,11 @@
       <c r="E35" s="13">
         <v>75.812386599726835</v>
       </c>
-      <c r="F35" s="105" t="s">
+      <c r="F35" s="106" t="s">
         <v>79</v>
       </c>
-      <c r="G35" s="104"/>
-      <c r="H35" s="104"/>
+      <c r="G35" s="107"/>
+      <c r="H35" s="107"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
@@ -7682,11 +7716,11 @@
       <c r="E36" s="13">
         <v>62.348001730346624</v>
       </c>
-      <c r="F36" s="105" t="s">
+      <c r="F36" s="106" t="s">
         <v>79</v>
       </c>
-      <c r="G36" s="104"/>
-      <c r="H36" s="104"/>
+      <c r="G36" s="107"/>
+      <c r="H36" s="107"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
@@ -7701,11 +7735,11 @@
       <c r="E37" s="13">
         <v>505.69965904746408</v>
       </c>
-      <c r="F37" s="105" t="s">
+      <c r="F37" s="106" t="s">
         <v>80</v>
       </c>
-      <c r="G37" s="104"/>
-      <c r="H37" s="104"/>
+      <c r="G37" s="107"/>
+      <c r="H37" s="107"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
@@ -7720,11 +7754,11 @@
       <c r="E38" s="13">
         <v>-138.34234368952491</v>
       </c>
-      <c r="F38" s="105" t="s">
+      <c r="F38" s="106" t="s">
         <v>78</v>
       </c>
-      <c r="G38" s="107"/>
-      <c r="H38" s="107"/>
+      <c r="G38" s="108"/>
+      <c r="H38" s="108"/>
     </row>
     <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
@@ -7739,11 +7773,11 @@
       <c r="E39" s="13">
         <v>-35.209092636503023</v>
       </c>
-      <c r="F39" s="105" t="s">
+      <c r="F39" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="G39" s="104"/>
-      <c r="H39" s="104"/>
+      <c r="G39" s="107"/>
+      <c r="H39" s="107"/>
     </row>
     <row r="40" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="18" t="s">
@@ -8126,11 +8160,11 @@
       <c r="B73" s="38"/>
     </row>
     <row r="74" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="97" t="s">
+      <c r="A74" s="99" t="s">
         <v>68</v>
       </c>
-      <c r="B74" s="98"/>
-      <c r="C74" s="99"/>
+      <c r="B74" s="100"/>
+      <c r="C74" s="101"/>
       <c r="D74" s="70" t="s">
         <v>1</v>
       </c>
@@ -8140,9 +8174,9 @@
       <c r="F74" s="7"/>
     </row>
     <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="100"/>
-      <c r="B75" s="101"/>
-      <c r="C75" s="102"/>
+      <c r="A75" s="102"/>
+      <c r="B75" s="103"/>
+      <c r="C75" s="104"/>
       <c r="D75" s="45" t="s">
         <v>53</v>
       </c>
@@ -8153,9 +8187,9 @@
       <c r="F75" s="7"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="100"/>
-      <c r="B76" s="101"/>
-      <c r="C76" s="102"/>
+      <c r="A76" s="102"/>
+      <c r="B76" s="103"/>
+      <c r="C76" s="104"/>
       <c r="D76" s="47" t="s">
         <v>54</v>
       </c>
@@ -8279,20 +8313,25 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="K4:O4"/>
-    <mergeCell ref="K11:O11"/>
-    <mergeCell ref="K22:O22"/>
-    <mergeCell ref="K29:O29"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="M30:O30"/>
-    <mergeCell ref="M31:O31"/>
-    <mergeCell ref="M32:O32"/>
-    <mergeCell ref="M33:O33"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="A74:C76"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
     <mergeCell ref="F36:H36"/>
     <mergeCell ref="F37:H37"/>
     <mergeCell ref="F38:H38"/>
@@ -8309,25 +8348,20 @@
     <mergeCell ref="M19:O19"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="A74:C76"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="M30:O30"/>
+    <mergeCell ref="M31:O31"/>
+    <mergeCell ref="M32:O32"/>
+    <mergeCell ref="M33:O33"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="K4:O4"/>
+    <mergeCell ref="K11:O11"/>
+    <mergeCell ref="K22:O22"/>
+    <mergeCell ref="K29:O29"/>
+    <mergeCell ref="M26:O26"/>
   </mergeCells>
   <conditionalFormatting sqref="A73:B73">
     <cfRule type="colorScale" priority="4">

</xml_diff>

<commit_message>
Tue, Nov  6, 2018  2:32:05 PM
</commit_message>
<xml_diff>
--- a/Data/Summary GDA.xlsx
+++ b/Data/Summary GDA.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robertsgr\Documents\MCH_Ischemia\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\groberts\Documents\MCH_Ischemia\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C751889-83CA-4563-B44B-D36C6720E459}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7590" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
@@ -295,7 +294,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -362,7 +361,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -845,12 +844,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -982,9 +992,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -994,7 +1001,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1275,11 +1290,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P71" workbookViewId="0">
-      <selection activeCell="X96" sqref="X96"/>
+    <sheetView topLeftCell="P7" workbookViewId="0">
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3340,7 +3355,7 @@
       <c r="R47" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="S47" s="11">
+      <c r="S47" s="68">
         <f>_xlfn.T.TEST(S5:S19,S26:S40,2,1)</f>
         <v>0.14860672439530109</v>
       </c>
@@ -3351,17 +3366,18 @@
         <f>_xlfn.T.TEST(V5:V8,V26:V29,2,1)</f>
         <v>0.50749319369333679</v>
       </c>
+      <c r="W47" s="111"/>
       <c r="X47" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="Y47" s="91">
+      <c r="Y47" s="96">
         <f>_xlfn.T.TEST(Y5:Y14,Y26:Y35,2,1)</f>
         <v>3.6498611111293301E-2</v>
       </c>
       <c r="AA47" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="AB47" s="29" t="e">
+      <c r="AB47" s="68" t="e">
         <f>_xlfn.T.TEST(AB5:AB9,AB26:AB30,2,1)</f>
         <v>#DIV/0!</v>
       </c>
@@ -3402,7 +3418,7 @@
       <c r="R48" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="S48" s="11">
+      <c r="S48" s="69">
         <f>(S41-S20)/SQRT((S42^2+S21^2)/2)</f>
         <v>0.27997081334390261</v>
       </c>
@@ -3413,17 +3429,18 @@
         <f>(V30-V9)/SQRT((V10^2+V31^2)/2)</f>
         <v>0.13214457906276661</v>
       </c>
+      <c r="W48" s="111"/>
       <c r="X48" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="Y48" s="109">
+      <c r="Y48" s="112">
         <f>(Y36-Y15)/SQRT((Y16^2+Y37^2)/2)</f>
         <v>0.56242970771187328</v>
       </c>
       <c r="AA48" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="AB48" s="32" t="e">
+      <c r="AB48" s="69" t="e">
         <f>(AB32-AB11)/AVERAGE(AB11,AB32)</f>
         <v>#DIV/0!</v>
       </c>
@@ -3432,6 +3449,7 @@
       <c r="M49" s="50"/>
       <c r="N49" s="16"/>
       <c r="P49" s="66"/>
+      <c r="V49" s="110"/>
       <c r="AA49" s="50"/>
       <c r="AB49" s="16"/>
     </row>
@@ -4784,7 +4802,7 @@
       <c r="Y84" s="79" t="s">
         <v>54</v>
       </c>
-      <c r="Z84" s="76">
+      <c r="Z84" s="81">
         <f>ABS((Y63-S68)/SQRT((Y64^2+S69^2)/2))</f>
         <v>0.10082381644472452</v>
       </c>
@@ -4796,6 +4814,7 @@
       <c r="U85" s="50"/>
       <c r="V85" s="16"/>
       <c r="W85" s="16"/>
+      <c r="Z85" s="109"/>
     </row>
     <row r="86" spans="2:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B86" s="99" t="s">
@@ -4943,7 +4962,7 @@
       <c r="U92" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="V92" s="76">
+      <c r="V92" s="73">
         <f>ABS((V30-Y36)/SQRT((V31^2+Y37^2)/2))</f>
         <v>0.34226865827209324</v>
       </c>
@@ -5003,7 +5022,7 @@
       <c r="U95" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="V95" s="81">
+      <c r="V95" s="73">
         <f>_xlfn.T.TEST(V53:V56,Y53:Y62,2,3)</f>
         <v>0.3268044085381886</v>
       </c>
@@ -5024,13 +5043,16 @@
       <c r="U96" s="82" t="s">
         <v>54</v>
       </c>
-      <c r="V96" s="76">
+      <c r="V96" s="81">
         <f>ABS((V57-Y63)/SQRT((V58^2+Y64^2)/2))</f>
         <v>0.50456471299066574</v>
       </c>
       <c r="W96" s="16"/>
     </row>
-    <row r="101" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V97" s="109"/>
+    </row>
+    <row r="101" spans="22:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B86:D88"/>
@@ -5100,7 +5122,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V57 Y63">
+  <conditionalFormatting sqref="Y63 V57">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="-100"/>
@@ -5141,11 +5163,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6819,7 +6841,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E57 H63">
+  <conditionalFormatting sqref="H63 E57">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="-100"/>
@@ -6861,11 +6883,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O96"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="K75" sqref="K75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6914,13 +6936,13 @@
         <v>63</v>
       </c>
       <c r="F4" s="7"/>
-      <c r="K4" s="105" t="s">
+      <c r="K4" s="108" t="s">
         <v>82</v>
       </c>
-      <c r="L4" s="105"/>
-      <c r="M4" s="105"/>
-      <c r="N4" s="105"/>
-      <c r="O4" s="105"/>
+      <c r="L4" s="108"/>
+      <c r="M4" s="108"/>
+      <c r="N4" s="108"/>
+      <c r="O4" s="108"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
@@ -6935,22 +6957,22 @@
       <c r="E5" s="13">
         <v>-204.41326846953166</v>
       </c>
-      <c r="F5" s="106" t="s">
+      <c r="F5" s="105" t="s">
         <v>73</v>
       </c>
-      <c r="G5" s="107"/>
-      <c r="H5" s="107"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="106"/>
       <c r="K5" s="95" t="s">
         <v>7</v>
       </c>
       <c r="L5" s="13">
         <v>-204.41326846953166</v>
       </c>
-      <c r="M5" s="106" t="s">
+      <c r="M5" s="105" t="s">
         <v>73</v>
       </c>
-      <c r="N5" s="107"/>
-      <c r="O5" s="107"/>
+      <c r="N5" s="106"/>
+      <c r="O5" s="106"/>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
@@ -6965,22 +6987,22 @@
       <c r="E6" s="13">
         <v>120.85244052933399</v>
       </c>
-      <c r="F6" s="106" t="s">
+      <c r="F6" s="105" t="s">
         <v>73</v>
       </c>
-      <c r="G6" s="107"/>
-      <c r="H6" s="107"/>
+      <c r="G6" s="106"/>
+      <c r="H6" s="106"/>
       <c r="K6" s="13" t="s">
         <v>12</v>
       </c>
       <c r="L6" s="13">
         <v>120.85244052933399</v>
       </c>
-      <c r="M6" s="106" t="s">
+      <c r="M6" s="105" t="s">
         <v>73</v>
       </c>
-      <c r="N6" s="107"/>
-      <c r="O6" s="107"/>
+      <c r="N6" s="106"/>
+      <c r="O6" s="106"/>
     </row>
     <row r="7" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
@@ -6995,54 +7017,54 @@
       <c r="E7" s="13">
         <v>-240.17138163193698</v>
       </c>
-      <c r="F7" s="106" t="s">
+      <c r="F7" s="105" t="s">
         <v>74</v>
       </c>
-      <c r="G7" s="107"/>
-      <c r="H7" s="107"/>
+      <c r="G7" s="106"/>
+      <c r="H7" s="106"/>
       <c r="K7" s="95" t="s">
         <v>43</v>
       </c>
       <c r="L7" s="13">
         <v>92.53518966457726</v>
       </c>
-      <c r="M7" s="106" t="s">
+      <c r="M7" s="105" t="s">
         <v>73</v>
       </c>
-      <c r="N7" s="107"/>
-      <c r="O7" s="107"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N7" s="106"/>
+      <c r="O7" s="106"/>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="13">
         <v>47.4720686969575</v>
       </c>
-      <c r="D8" s="93" t="s">
+      <c r="D8" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="114">
         <v>937.89820907570538</v>
       </c>
-      <c r="F8" s="106" t="s">
+      <c r="F8" s="105" t="s">
         <v>80</v>
       </c>
-      <c r="G8" s="107"/>
-      <c r="H8" s="107"/>
+      <c r="G8" s="106"/>
+      <c r="H8" s="106"/>
       <c r="K8" s="13" t="s">
         <v>45</v>
       </c>
       <c r="L8" s="13">
         <v>91.563377374129416</v>
       </c>
-      <c r="M8" s="106" t="s">
+      <c r="M8" s="105" t="s">
         <v>73</v>
       </c>
-      <c r="N8" s="107"/>
-      <c r="O8" s="107"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N8" s="106"/>
+      <c r="O8" s="106"/>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
@@ -7055,11 +7077,11 @@
       <c r="E9" s="13">
         <v>110.27258157435739</v>
       </c>
-      <c r="F9" s="106" t="s">
+      <c r="F9" s="105" t="s">
         <v>76</v>
       </c>
-      <c r="G9" s="107"/>
-      <c r="H9" s="107"/>
+      <c r="G9" s="106"/>
+      <c r="H9" s="106"/>
       <c r="K9" s="50"/>
       <c r="L9" s="50"/>
       <c r="M9" s="98"/>
@@ -7098,13 +7120,13 @@
       <c r="E11" s="13">
         <v>89.698925848177623</v>
       </c>
-      <c r="K11" s="105" t="s">
+      <c r="K11" s="108" t="s">
         <v>83</v>
       </c>
-      <c r="L11" s="105"/>
-      <c r="M11" s="105"/>
-      <c r="N11" s="105"/>
-      <c r="O11" s="105"/>
+      <c r="L11" s="108"/>
+      <c r="M11" s="108"/>
+      <c r="N11" s="108"/>
+      <c r="O11" s="108"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
@@ -7119,22 +7141,22 @@
       <c r="E12" s="13">
         <v>86.300113483264099</v>
       </c>
-      <c r="F12" s="106" t="s">
+      <c r="F12" s="105" t="s">
         <v>77</v>
       </c>
-      <c r="G12" s="107"/>
-      <c r="H12" s="107"/>
+      <c r="G12" s="106"/>
+      <c r="H12" s="106"/>
       <c r="K12" s="94" t="s">
         <v>36</v>
       </c>
       <c r="L12" s="13">
         <v>-131.89988980258138</v>
       </c>
-      <c r="M12" s="106" t="s">
+      <c r="M12" s="105" t="s">
         <v>78</v>
       </c>
-      <c r="N12" s="107"/>
-      <c r="O12" s="107"/>
+      <c r="N12" s="106"/>
+      <c r="O12" s="106"/>
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
@@ -7149,22 +7171,22 @@
       <c r="E13" s="13">
         <v>-166.94515408677509</v>
       </c>
-      <c r="F13" s="106" t="s">
+      <c r="F13" s="105" t="s">
         <v>78</v>
       </c>
-      <c r="G13" s="107"/>
-      <c r="H13" s="107"/>
+      <c r="G13" s="106"/>
+      <c r="H13" s="106"/>
       <c r="K13" s="94" t="s">
         <v>36</v>
       </c>
       <c r="L13" s="13">
         <v>-35.209092636503023</v>
       </c>
-      <c r="M13" s="106" t="s">
+      <c r="M13" s="105" t="s">
         <v>78</v>
       </c>
-      <c r="N13" s="107"/>
-      <c r="O13" s="107"/>
+      <c r="N13" s="106"/>
+      <c r="O13" s="106"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
@@ -7179,22 +7201,22 @@
       <c r="E14" s="13">
         <v>-92.575768832528084</v>
       </c>
-      <c r="F14" s="106" t="s">
+      <c r="F14" s="105" t="s">
         <v>79</v>
       </c>
-      <c r="G14" s="107"/>
-      <c r="H14" s="107"/>
+      <c r="G14" s="106"/>
+      <c r="H14" s="106"/>
       <c r="K14" s="93" t="s">
         <v>34</v>
       </c>
       <c r="L14" s="13">
         <v>-236.73173748573311</v>
       </c>
-      <c r="M14" s="106" t="s">
+      <c r="M14" s="105" t="s">
         <v>78</v>
       </c>
-      <c r="N14" s="108"/>
-      <c r="O14" s="108"/>
+      <c r="N14" s="107"/>
+      <c r="O14" s="107"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
@@ -7209,22 +7231,22 @@
       <c r="E15" s="13">
         <v>-83.419333217354989</v>
       </c>
-      <c r="F15" s="106" t="s">
+      <c r="F15" s="105" t="s">
         <v>79</v>
       </c>
-      <c r="G15" s="107"/>
-      <c r="H15" s="107"/>
+      <c r="G15" s="106"/>
+      <c r="H15" s="106"/>
       <c r="K15" s="93" t="s">
         <v>55</v>
       </c>
       <c r="L15" s="13">
         <v>-138.34234368952491</v>
       </c>
-      <c r="M15" s="106" t="s">
+      <c r="M15" s="105" t="s">
         <v>78</v>
       </c>
-      <c r="N15" s="108"/>
-      <c r="O15" s="108"/>
+      <c r="N15" s="107"/>
+      <c r="O15" s="107"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
@@ -7239,22 +7261,22 @@
       <c r="E16" s="13">
         <v>133.54048634274659</v>
       </c>
-      <c r="F16" s="106" t="s">
+      <c r="F16" s="105" t="s">
         <v>81</v>
       </c>
-      <c r="G16" s="107"/>
-      <c r="H16" s="107"/>
+      <c r="G16" s="106"/>
+      <c r="H16" s="106"/>
       <c r="K16" s="93" t="s">
         <v>27</v>
       </c>
       <c r="L16" s="13">
         <v>-166.94515408677509</v>
       </c>
-      <c r="M16" s="106" t="s">
+      <c r="M16" s="105" t="s">
         <v>78</v>
       </c>
-      <c r="N16" s="107"/>
-      <c r="O16" s="107"/>
+      <c r="N16" s="106"/>
+      <c r="O16" s="106"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
@@ -7269,22 +7291,22 @@
       <c r="E17" s="13">
         <v>-236.73173748573311</v>
       </c>
-      <c r="F17" s="106" t="s">
+      <c r="F17" s="105" t="s">
         <v>78</v>
       </c>
-      <c r="G17" s="108"/>
-      <c r="H17" s="108"/>
+      <c r="G17" s="107"/>
+      <c r="H17" s="107"/>
       <c r="K17" s="93" t="s">
         <v>27</v>
       </c>
       <c r="L17" s="13">
         <v>-183.3714839935835</v>
       </c>
-      <c r="M17" s="106" t="s">
+      <c r="M17" s="105" t="s">
         <v>78</v>
       </c>
-      <c r="N17" s="107"/>
-      <c r="O17" s="107"/>
+      <c r="N17" s="106"/>
+      <c r="O17" s="106"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
@@ -7299,22 +7321,22 @@
       <c r="E18" s="13">
         <v>-131.89988980258138</v>
       </c>
-      <c r="F18" s="106" t="s">
+      <c r="F18" s="105" t="s">
         <v>76</v>
       </c>
-      <c r="G18" s="107"/>
-      <c r="H18" s="107"/>
+      <c r="G18" s="106"/>
+      <c r="H18" s="106"/>
       <c r="K18" s="13" t="s">
         <v>9</v>
       </c>
       <c r="L18" s="13">
         <v>110.27258157435739</v>
       </c>
-      <c r="M18" s="106" t="s">
+      <c r="M18" s="105" t="s">
         <v>76</v>
       </c>
-      <c r="N18" s="107"/>
-      <c r="O18" s="107"/>
+      <c r="N18" s="106"/>
+      <c r="O18" s="106"/>
     </row>
     <row r="19" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
@@ -7335,11 +7357,11 @@
       <c r="L19" s="13">
         <v>361.1808928803157</v>
       </c>
-      <c r="M19" s="106" t="s">
+      <c r="M19" s="105" t="s">
         <v>76</v>
       </c>
-      <c r="N19" s="107"/>
-      <c r="O19" s="107"/>
+      <c r="N19" s="106"/>
+      <c r="O19" s="106"/>
     </row>
     <row r="20" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
@@ -7385,13 +7407,13 @@
         <v>14</v>
       </c>
       <c r="F22" s="7"/>
-      <c r="K22" s="105" t="s">
+      <c r="K22" s="108" t="s">
         <v>84</v>
       </c>
-      <c r="L22" s="105"/>
-      <c r="M22" s="105"/>
-      <c r="N22" s="105"/>
-      <c r="O22" s="105"/>
+      <c r="L22" s="108"/>
+      <c r="M22" s="108"/>
+      <c r="N22" s="108"/>
+      <c r="O22" s="108"/>
     </row>
     <row r="23" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="21"/>
@@ -7403,11 +7425,11 @@
       <c r="L23" s="13">
         <v>86.300113483264099</v>
       </c>
-      <c r="M23" s="106" t="s">
+      <c r="M23" s="105" t="s">
         <v>77</v>
       </c>
-      <c r="N23" s="107"/>
-      <c r="O23" s="107"/>
+      <c r="N23" s="106"/>
+      <c r="O23" s="106"/>
     </row>
     <row r="24" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
@@ -7424,11 +7446,11 @@
       <c r="L24" s="13">
         <v>110.95469137218241</v>
       </c>
-      <c r="M24" s="106" t="s">
+      <c r="M24" s="105" t="s">
         <v>77</v>
       </c>
-      <c r="N24" s="107"/>
-      <c r="O24" s="107"/>
+      <c r="N24" s="106"/>
+      <c r="O24" s="106"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
@@ -7450,11 +7472,11 @@
       <c r="L25" s="13">
         <v>133.54048634274659</v>
       </c>
-      <c r="M25" s="106" t="s">
+      <c r="M25" s="105" t="s">
         <v>81</v>
       </c>
-      <c r="N25" s="107"/>
-      <c r="O25" s="107"/>
+      <c r="N25" s="106"/>
+      <c r="O25" s="106"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
@@ -7469,22 +7491,22 @@
       <c r="E26" s="13">
         <v>92.53518966457726</v>
       </c>
-      <c r="F26" s="106" t="s">
+      <c r="F26" s="105" t="s">
         <v>73</v>
       </c>
-      <c r="G26" s="107"/>
-      <c r="H26" s="107"/>
+      <c r="G26" s="106"/>
+      <c r="H26" s="106"/>
       <c r="K26" s="93" t="s">
         <v>33</v>
       </c>
       <c r="L26" s="13">
         <v>505.69965904746408</v>
       </c>
-      <c r="M26" s="106" t="s">
+      <c r="M26" s="105" t="s">
         <v>80</v>
       </c>
-      <c r="N26" s="107"/>
-      <c r="O26" s="107"/>
+      <c r="N26" s="106"/>
+      <c r="O26" s="106"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
@@ -7499,11 +7521,11 @@
       <c r="E27" s="13">
         <v>91.563377374129416</v>
       </c>
-      <c r="F27" s="106" t="s">
+      <c r="F27" s="105" t="s">
         <v>73</v>
       </c>
-      <c r="G27" s="107"/>
-      <c r="H27" s="107"/>
+      <c r="G27" s="106"/>
+      <c r="H27" s="106"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
@@ -7518,39 +7540,39 @@
       <c r="E28" s="13">
         <v>-149.34216837262221</v>
       </c>
-      <c r="F28" s="106" t="s">
+      <c r="F28" s="105" t="s">
         <v>74</v>
       </c>
-      <c r="G28" s="107"/>
-      <c r="H28" s="107"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G28" s="106"/>
+      <c r="H28" s="106"/>
+    </row>
+    <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B29" s="13">
         <v>69.643553114048373</v>
       </c>
-      <c r="D29" s="93" t="s">
+      <c r="D29" s="113" t="s">
         <v>49</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="114">
         <v>839.46341018580051</v>
       </c>
-      <c r="F29" s="106" t="s">
+      <c r="F29" s="105" t="s">
         <v>75</v>
       </c>
-      <c r="G29" s="107"/>
-      <c r="H29" s="107"/>
-      <c r="K29" s="105" t="s">
+      <c r="G29" s="106"/>
+      <c r="H29" s="106"/>
+      <c r="K29" s="108" t="s">
         <v>85</v>
       </c>
-      <c r="L29" s="105"/>
-      <c r="M29" s="105"/>
-      <c r="N29" s="105"/>
-      <c r="O29" s="105"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L29" s="108"/>
+      <c r="M29" s="108"/>
+      <c r="N29" s="108"/>
+      <c r="O29" s="108"/>
+    </row>
+    <row r="30" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>15</v>
       </c>
@@ -7564,22 +7586,22 @@
       <c r="E30" s="13">
         <v>361.1808928803157</v>
       </c>
-      <c r="F30" s="106" t="s">
+      <c r="F30" s="105" t="s">
         <v>76</v>
       </c>
-      <c r="G30" s="107"/>
-      <c r="H30" s="107"/>
+      <c r="G30" s="106"/>
+      <c r="H30" s="106"/>
       <c r="K30" s="13" t="s">
         <v>29</v>
       </c>
       <c r="L30" s="13">
         <v>-92.575768832528084</v>
       </c>
-      <c r="M30" s="106" t="s">
+      <c r="M30" s="105" t="s">
         <v>79</v>
       </c>
-      <c r="N30" s="107"/>
-      <c r="O30" s="107"/>
+      <c r="N30" s="106"/>
+      <c r="O30" s="106"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
@@ -7601,11 +7623,11 @@
       <c r="L31" s="13">
         <v>75.812386599726835</v>
       </c>
-      <c r="M31" s="106" t="s">
+      <c r="M31" s="105" t="s">
         <v>79</v>
       </c>
-      <c r="N31" s="107"/>
-      <c r="O31" s="107"/>
+      <c r="N31" s="106"/>
+      <c r="O31" s="106"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
@@ -7627,11 +7649,11 @@
       <c r="L32" s="13">
         <v>-83.419333217354989</v>
       </c>
-      <c r="M32" s="106" t="s">
+      <c r="M32" s="105" t="s">
         <v>79</v>
       </c>
-      <c r="N32" s="107"/>
-      <c r="O32" s="107"/>
+      <c r="N32" s="106"/>
+      <c r="O32" s="106"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
@@ -7647,22 +7669,22 @@
       <c r="E33" s="13">
         <v>110.95469137218241</v>
       </c>
-      <c r="F33" s="106" t="s">
+      <c r="F33" s="105" t="s">
         <v>77</v>
       </c>
-      <c r="G33" s="107"/>
-      <c r="H33" s="107"/>
+      <c r="G33" s="106"/>
+      <c r="H33" s="106"/>
       <c r="K33" s="13" t="s">
         <v>31</v>
       </c>
       <c r="L33" s="13">
         <v>62.348001730346624</v>
       </c>
-      <c r="M33" s="106" t="s">
+      <c r="M33" s="105" t="s">
         <v>79</v>
       </c>
-      <c r="N33" s="107"/>
-      <c r="O33" s="107"/>
+      <c r="N33" s="106"/>
+      <c r="O33" s="106"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
@@ -7678,11 +7700,11 @@
       <c r="E34" s="13">
         <v>-183.3714839935835</v>
       </c>
-      <c r="F34" s="106" t="s">
+      <c r="F34" s="105" t="s">
         <v>78</v>
       </c>
-      <c r="G34" s="107"/>
-      <c r="H34" s="107"/>
+      <c r="G34" s="106"/>
+      <c r="H34" s="106"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
@@ -7697,11 +7719,11 @@
       <c r="E35" s="13">
         <v>75.812386599726835</v>
       </c>
-      <c r="F35" s="106" t="s">
+      <c r="F35" s="105" t="s">
         <v>79</v>
       </c>
-      <c r="G35" s="107"/>
-      <c r="H35" s="107"/>
+      <c r="G35" s="106"/>
+      <c r="H35" s="106"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
@@ -7716,11 +7738,11 @@
       <c r="E36" s="13">
         <v>62.348001730346624</v>
       </c>
-      <c r="F36" s="106" t="s">
+      <c r="F36" s="105" t="s">
         <v>79</v>
       </c>
-      <c r="G36" s="107"/>
-      <c r="H36" s="107"/>
+      <c r="G36" s="106"/>
+      <c r="H36" s="106"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
@@ -7735,11 +7757,11 @@
       <c r="E37" s="13">
         <v>505.69965904746408</v>
       </c>
-      <c r="F37" s="106" t="s">
+      <c r="F37" s="105" t="s">
         <v>80</v>
       </c>
-      <c r="G37" s="107"/>
-      <c r="H37" s="107"/>
+      <c r="G37" s="106"/>
+      <c r="H37" s="106"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
@@ -7754,11 +7776,11 @@
       <c r="E38" s="13">
         <v>-138.34234368952491</v>
       </c>
-      <c r="F38" s="106" t="s">
+      <c r="F38" s="105" t="s">
         <v>78</v>
       </c>
-      <c r="G38" s="108"/>
-      <c r="H38" s="108"/>
+      <c r="G38" s="107"/>
+      <c r="H38" s="107"/>
     </row>
     <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
@@ -7773,11 +7795,11 @@
       <c r="E39" s="13">
         <v>-35.209092636503023</v>
       </c>
-      <c r="F39" s="106" t="s">
+      <c r="F39" s="105" t="s">
         <v>76</v>
       </c>
-      <c r="G39" s="107"/>
-      <c r="H39" s="107"/>
+      <c r="G39" s="106"/>
+      <c r="H39" s="106"/>
     </row>
     <row r="40" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="18" t="s">
@@ -8313,11 +8335,34 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="K4:O4"/>
+    <mergeCell ref="K11:O11"/>
+    <mergeCell ref="K22:O22"/>
+    <mergeCell ref="K29:O29"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="M32:O32"/>
+    <mergeCell ref="M33:O33"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="M30:O30"/>
+    <mergeCell ref="M31:O31"/>
     <mergeCell ref="F35:H35"/>
     <mergeCell ref="A74:C76"/>
     <mergeCell ref="F5:H5"/>
@@ -8334,34 +8379,11 @@
     <mergeCell ref="F18:H18"/>
     <mergeCell ref="F36:H36"/>
     <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="M30:O30"/>
-    <mergeCell ref="M31:O31"/>
-    <mergeCell ref="M32:O32"/>
-    <mergeCell ref="M33:O33"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="K4:O4"/>
-    <mergeCell ref="K11:O11"/>
-    <mergeCell ref="K22:O22"/>
-    <mergeCell ref="K29:O29"/>
-    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
   </mergeCells>
   <conditionalFormatting sqref="A73:B73">
     <cfRule type="colorScale" priority="4">

</xml_diff>